<commit_message>
main_loop ver.1.0: including fuel cost analysis
</commit_message>
<xml_diff>
--- a/input/data/INPUT.xlsx
+++ b/input/data/INPUT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\KHT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\1. econ\1. code\ECON_0127_v2\input\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{373E73BB-678E-43C0-8982-A9C31EC779FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B54F4D-4B69-4253-95FE-6258ADA9147B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{9F0F0BF7-5D50-3A46-9D53-789F70DB3A62}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9F0F0BF7-5D50-3A46-9D53-789F70DB3A62}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -189,9 +189,6 @@
     <t>$/SWU</t>
   </si>
   <si>
-    <t>$/tU</t>
-  </si>
-  <si>
     <t>months</t>
   </si>
   <si>
@@ -246,28 +243,33 @@
     <t>COSTperHM</t>
   </si>
   <si>
+    <t>ASSEMBLYperCORE</t>
+  </si>
+  <si>
+    <t>yearsForInterimStorage</t>
+  </si>
+  <si>
+    <t>$M (8-12)</t>
+  </si>
+  <si>
+    <t>60-80$/HMkg</t>
+  </si>
+  <si>
+    <t>HMton per Assembly</t>
+  </si>
+  <si>
+    <t>interimCOST_OM</t>
+  </si>
+  <si>
+    <t>$M (annualy)</t>
+  </si>
+  <si>
+    <t>$/kgU</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
     <t>HMperASSEMBLY</t>
-  </si>
-  <si>
-    <t>ASSEMBLYperCORE</t>
-  </si>
-  <si>
-    <t>yearsForInterimStorage</t>
-  </si>
-  <si>
-    <t>$M (8-12)</t>
-  </si>
-  <si>
-    <t>60-80$/HMkg</t>
-  </si>
-  <si>
-    <t>HMton per Assembly</t>
-  </si>
-  <si>
-    <t>interimCOST_OM</t>
-  </si>
-  <si>
-    <t>$M (annualy)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -312,12 +314,16 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="0" tint="-0.499984740745262"/>
       <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -325,6 +331,8 @@
       <sz val="12"/>
       <color theme="0" tint="-0.499984740745262"/>
       <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -332,6 +340,8 @@
       <sz val="12"/>
       <color theme="3" tint="0.249977111117893"/>
       <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -340,6 +350,8 @@
       <sz val="12"/>
       <color theme="3" tint="0.249977111117893"/>
       <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1011,8 +1023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D383CB1-5121-284F-8EFF-BAAEA81D92DF}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="17.25"/>
@@ -1058,7 +1070,7 @@
         <v>0.78800000000000003</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1082,7 +1094,7 @@
         <v>0.26100000000000001</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1094,7 +1106,7 @@
         <v>0.35</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="18" thickBot="1">
@@ -1120,7 +1132,7 @@
         <v>7.11E-3</v>
       </c>
       <c r="D8" s="58" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1132,7 +1144,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1144,7 +1156,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="D10" s="59" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1192,7 +1204,7 @@
         <v>350</v>
       </c>
       <c r="D14" s="59" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1204,7 +1216,7 @@
         <v>12</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1216,7 +1228,7 @@
         <v>2.5</v>
       </c>
       <c r="D16" s="59" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1228,7 +1240,7 @@
         <v>18</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1240,61 +1252,61 @@
         <v>1</v>
       </c>
       <c r="D18" s="59" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="71"/>
       <c r="B19" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C19" s="52">
         <v>9</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="71"/>
       <c r="B20" s="66" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C20" s="56">
         <v>0.75</v>
       </c>
       <c r="D20" s="59" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="71"/>
       <c r="B21" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C21" s="52">
         <v>70</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="71"/>
       <c r="B22" s="66" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="C22" s="56">
         <v>0.45</v>
       </c>
       <c r="D22" s="59" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="71"/>
       <c r="B23" s="10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C23" s="52">
         <v>241</v>
@@ -1306,7 +1318,7 @@
     <row r="24" spans="1:4" ht="18" thickBot="1">
       <c r="A24" s="72"/>
       <c r="B24" s="67" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C24" s="60">
         <v>5</v>
@@ -1352,7 +1364,7 @@
         <v>0.9</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1376,7 +1388,7 @@
         <v>0.8</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1390,7 +1402,7 @@
         <v>0</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1402,7 +1414,7 @@
         <v>0.05</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1414,7 +1426,7 @@
         <v>0.05</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1426,7 +1438,7 @@
         <v>0.1</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1438,7 +1450,7 @@
         <v>0.05</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1450,7 +1462,7 @@
         <v>0.05</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1462,7 +1474,7 @@
         <v>0.05</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1474,7 +1486,7 @@
         <v>0.7</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1486,7 +1498,7 @@
         <v>0.05</v>
       </c>
       <c r="D38" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1522,7 +1534,7 @@
         <v>0.22</v>
       </c>
       <c r="D41" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="18" thickBot="1">
@@ -1534,29 +1546,29 @@
         <v>0.05</v>
       </c>
       <c r="D42" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="18" thickBot="1">
       <c r="A43" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B43" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="B43" s="19" t="s">
+      <c r="C43" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="C43" s="44" t="s">
+      <c r="D43" s="32" t="s">
         <v>56</v>
-      </c>
-      <c r="D43" s="32" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B44" s="27" t="s">
         <v>58</v>
-      </c>
-      <c r="B44" s="27" t="s">
-        <v>59</v>
       </c>
       <c r="C44" s="45">
         <v>1</v>
@@ -1566,7 +1578,7 @@
     <row r="45" spans="1:4">
       <c r="A45" s="24"/>
       <c r="B45" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C45" s="46">
         <v>1</v>
@@ -1576,7 +1588,7 @@
     <row r="46" spans="1:4">
       <c r="A46" s="24"/>
       <c r="B46" s="28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C46" s="47">
         <v>1</v>
@@ -1586,7 +1598,7 @@
     <row r="47" spans="1:4">
       <c r="A47" s="24"/>
       <c r="B47" s="30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C47" s="46">
         <v>1</v>
@@ -1596,7 +1608,7 @@
     <row r="48" spans="1:4" ht="18" thickBot="1">
       <c r="A48" s="25"/>
       <c r="B48" s="29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C48" s="48">
         <v>1</v>
@@ -1605,13 +1617,13 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B49" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="B49" s="26" t="s">
-        <v>64</v>
-      </c>
       <c r="C49" s="47" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>